<commit_message>
Jenkins parameterized build completed
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="addCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -36,6 +36,9 @@
     <t xml:space="preserve">alertText</t>
   </si>
   <si>
+    <t xml:space="preserve">Runmode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raman</t>
   </si>
   <si>
@@ -48,12 +51,18 @@
     <t xml:space="preserve">Customer added successfully</t>
   </si>
   <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rahul</t>
   </si>
   <si>
     <t xml:space="preserve">priyanka</t>
   </si>
   <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
     <t xml:space="preserve">kamal</t>
   </si>
   <si>
@@ -81,9 +90,6 @@
     <t xml:space="preserve">TC_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Runmode</t>
-  </si>
-  <si>
     <t xml:space="preserve">BankManagerLoginTest</t>
   </si>
   <si>
@@ -94,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">OpenAccountTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
   </si>
 </sst>
 </file>
@@ -208,13 +211,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.57"/>
   </cols>
@@ -232,61 +235,76 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
+      <c r="E3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -311,25 +329,25 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -350,11 +368,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.13"/>
@@ -362,34 +380,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>